<commit_message>
Remove most schema rows marked to be removed
</commit_message>
<xml_diff>
--- a/schema.xlsx
+++ b/schema.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drewl\Documents\GitHub\food-access-map-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e3f8cbb5d9583421/Desktop/FAM_MASTER/food-access-map-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20759C7-350E-4C0B-9877-DF21971DD0AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{E20759C7-350E-4C0B-9877-DF21971DD0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA63972C-16EF-4A97-9F7D-7E87441D2B17}"/>
   <bookViews>
-    <workbookView xWindow="31380" yWindow="2325" windowWidth="21600" windowHeight="11955" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master_table" sheetId="1" r:id="rId1"/>
     <sheet name="open_hours" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">master_table!$A$1:$D$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">master_table!$A$1:$D$28</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
   <si>
     <t>field</t>
   </si>
@@ -55,15 +55,6 @@
     <t>address</t>
   </si>
   <si>
-    <t>street_one</t>
-  </si>
-  <si>
-    <t>Some food sources are on street corners and not at a specific address</t>
-  </si>
-  <si>
-    <t>street_two</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
@@ -91,45 +82,9 @@
     <t>date_to</t>
   </si>
   <si>
-    <t>open_time1</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>close_time1</t>
-  </si>
-  <si>
-    <t>open_time2</t>
-  </si>
-  <si>
-    <t>close_time2</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
     <t>bool (1=yes, 0=no)</t>
   </si>
   <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
     <t>SNAP</t>
   </si>
   <si>
@@ -214,9 +169,6 @@
     <t>Farmer's Market Nutrition Program</t>
   </si>
   <si>
-    <t>remove - put in Address instead</t>
-  </si>
-  <si>
     <t>REMOVE - move to a GIS table</t>
   </si>
   <si>
@@ -269,9 +221,6 @@
   </si>
   <si>
     <t>rename from "fresh_produce-healthy"</t>
-  </si>
-  <si>
-    <t>eliminate - move to open_hours</t>
   </si>
   <si>
     <t>data_issues</t>
@@ -327,11 +276,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
@@ -673,11 +621,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1003"/>
+  <dimension ref="A1:D990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -701,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
@@ -712,52 +660,52 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>48</v>
+        <v>32</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1">
@@ -768,10 +716,10 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1">
@@ -782,7 +730,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1">
@@ -793,451 +741,304 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>48</v>
+      <c r="D12" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>48</v>
+        <v>54</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>48</v>
+        <v>35</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="4" t="s">
         <v>48</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>79</v>
+        <v>21</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>48</v>
+        <v>60</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>73</v>
+        <v>58</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>48</v>
+        <v>65</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A31" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A32" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A34" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A35" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A37" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A38" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A39" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A40" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A42" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:4" ht="14.25" customHeight="1"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -2180,21 +1981,8 @@
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
     <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
-    <row r="1002" ht="14.25" customHeight="1"/>
-    <row r="1003" ht="14.25" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:D41" xr:uid="{F0E35ADD-0666-4F3B-AAA1-A37AC3395626}"/>
+  <autoFilter ref="A1:D28" xr:uid="{F0E35ADD-0666-4F3B-AAA1-A37AC3395626}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <extLst>
@@ -2239,51 +2027,51 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove MRFEI Score row
</commit_message>
<xml_diff>
--- a/schema.xlsx
+++ b/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e3f8cbb5d9583421/Desktop/FAM_MASTER/food-access-map-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{E20759C7-350E-4C0B-9877-DF21971DD0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA63972C-16EF-4A97-9F7D-7E87441D2B17}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{E20759C7-350E-4C0B-9877-DF21971DD0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EE02888-0C9F-4449-B648-EAB8E591D0A7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="63">
   <si>
     <t>field</t>
   </si>
@@ -97,12 +97,6 @@
     <t>possibly unnecessary field if we assume specific types of food sources have fresh produce</t>
   </si>
   <si>
-    <t>MRFEI_score</t>
-  </si>
-  <si>
-    <t>score out of 100</t>
-  </si>
-  <si>
     <t>latitude</t>
   </si>
   <si>
@@ -167,9 +161,6 @@
   </si>
   <si>
     <t>Farmer's Market Nutrition Program</t>
-  </si>
-  <si>
-    <t>REMOVE - move to a GIS table</t>
   </si>
   <si>
     <t>latlng_source</t>
@@ -244,18 +235,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -276,12 +261,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,11 +605,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D990"/>
+  <dimension ref="A1:D989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -649,7 +633,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
@@ -660,52 +644,52 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>49</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1">
@@ -716,10 +700,10 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1">
@@ -730,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1">
@@ -741,7 +725,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1">
@@ -752,7 +736,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1">
@@ -763,7 +747,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1">
@@ -774,18 +758,18 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>33</v>
+      <c r="D12" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1">
@@ -799,77 +783,77 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>33</v>
+        <v>51</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="3" t="s">
         <v>33</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>33</v>
+        <v>45</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
@@ -883,7 +867,7 @@
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
@@ -897,7 +881,7 @@
         <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
@@ -908,7 +892,7 @@
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
@@ -919,7 +903,7 @@
         <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1">
@@ -930,15 +914,15 @@
         <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
@@ -946,80 +930,67 @@
       <c r="C24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>63</v>
+      <c r="D24" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>33</v>
+        <v>57</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A29" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
+        <v>62</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:4" ht="14.25" customHeight="1"/>
@@ -1980,7 +1951,6 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A1:D28" xr:uid="{F0E35ADD-0666-4F3B-AAA1-A37AC3395626}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -2027,51 +1997,51 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add basic checks and tests for checks
</commit_message>
<xml_diff>
--- a/schema.xlsx
+++ b/schema.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drewl\Documents\GitHub\food-access-map-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e3f8cbb5d9583421/Desktop/FAM_MASTER/food-access-map-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20759C7-350E-4C0B-9877-DF21971DD0AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{E20759C7-350E-4C0B-9877-DF21971DD0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BAB5A80-2E76-40D2-A30C-C7626B033DFA}"/>
   <bookViews>
-    <workbookView xWindow="31380" yWindow="2325" windowWidth="21600" windowHeight="11955" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="16845" windowHeight="12150" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master_table" sheetId="1" r:id="rId1"/>
     <sheet name="open_hours" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">master_table!$A$1:$D$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">master_table!$A$1:$D$28</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="63">
   <si>
     <t>field</t>
   </si>
@@ -55,15 +55,6 @@
     <t>address</t>
   </si>
   <si>
-    <t>street_one</t>
-  </si>
-  <si>
-    <t>Some food sources are on street corners and not at a specific address</t>
-  </si>
-  <si>
-    <t>street_two</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
@@ -91,45 +82,9 @@
     <t>date_to</t>
   </si>
   <si>
-    <t>open_time1</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>close_time1</t>
-  </si>
-  <si>
-    <t>open_time2</t>
-  </si>
-  <si>
-    <t>close_time2</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
     <t>bool (1=yes, 0=no)</t>
   </si>
   <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
     <t>SNAP</t>
   </si>
   <si>
@@ -142,12 +97,6 @@
     <t>possibly unnecessary field if we assume specific types of food sources have fresh produce</t>
   </si>
   <si>
-    <t>MRFEI_score</t>
-  </si>
-  <si>
-    <t>score out of 100</t>
-  </si>
-  <si>
     <t>latitude</t>
   </si>
   <si>
@@ -214,12 +163,6 @@
     <t>Farmer's Market Nutrition Program</t>
   </si>
   <si>
-    <t>remove - put in Address instead</t>
-  </si>
-  <si>
-    <t>REMOVE - move to a GIS table</t>
-  </si>
-  <si>
     <t>latlng_source</t>
   </si>
   <si>
@@ -269,9 +212,6 @@
   </si>
   <si>
     <t>rename from "fresh_produce-healthy"</t>
-  </si>
-  <si>
-    <t>eliminate - move to open_hours</t>
   </si>
   <si>
     <t>data_issues</t>
@@ -295,18 +235,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -327,13 +261,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,11 +605,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1003"/>
+  <dimension ref="A1:D989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29:XFD989"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -701,7 +633,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
@@ -712,52 +644,52 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="4" t="s">
         <v>48</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>48</v>
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1">
@@ -768,10 +700,10 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1">
@@ -782,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1">
@@ -793,451 +725,291 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>48</v>
+      <c r="D12" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>48</v>
+        <v>33</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>79</v>
+        <v>21</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>48</v>
+        <v>57</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>73</v>
+        <v>55</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A31" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A32" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A34" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A35" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A37" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A38" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A39" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A42" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:4" ht="14.25" customHeight="1"/>
+    </row>
+    <row r="29" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -2179,22 +1951,8 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
-    <row r="1002" ht="14.25" customHeight="1"/>
-    <row r="1003" ht="14.25" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:D41" xr:uid="{F0E35ADD-0666-4F3B-AAA1-A37AC3395626}"/>
+  <autoFilter ref="A1:D28" xr:uid="{F0E35ADD-0666-4F3B-AAA1-A37AC3395626}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <extLst>
@@ -2239,51 +1997,51 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>